<commit_message>
Uptaded experiment (training-test 2016-2019) - Updated script 'run_experiment_training_test_2016_2019.m' - Updated script 'plot_compare_obs_pred.m' - Updated script 'plot_results.m' - Load updated dataset - Load updated results
</commit_message>
<xml_diff>
--- a/Parameters-Estimation/Salinity_Estimation/1-Trained-Models/training_test_2016_2019/Results-salinity-calibration-model-k-10.xlsx
+++ b/Parameters-Estimation/Salinity_Estimation/1-Trained-Models/training_test_2016_2019/Results-salinity-calibration-model-k-10.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Row</t>
   </si>
@@ -30,37 +30,7 @@
     <t>RMSE</t>
   </si>
   <si>
-    <t>MAE</t>
-  </si>
-  <si>
-    <t>RSE</t>
-  </si>
-  <si>
-    <t>RRSE</t>
-  </si>
-  <si>
-    <t>RAE</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>Corr Coeff</t>
-  </si>
-  <si>
-    <t>Row</t>
-  </si>
-  <si>
-    <t>random_forest</t>
-  </si>
-  <si>
-    <t>lsboost</t>
-  </si>
-  <si>
-    <t>neural_network</t>
-  </si>
-  <si>
-    <t>RMSE</t>
+    <t>NRMSE</t>
   </si>
   <si>
     <t>MAE</t>
@@ -124,121 +94,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="true"/>
     <col min="2" max="2" width="11.7109375" customWidth="true"/>
-    <col min="3" max="3" width="11.7109375" customWidth="true"/>
-    <col min="4" max="4" width="12.7109375" customWidth="true"/>
+    <col min="3" max="3" width="12.7109375" customWidth="true"/>
+    <col min="4" max="4" width="11.7109375" customWidth="true"/>
     <col min="5" max="5" width="12.7109375" customWidth="true"/>
     <col min="6" max="6" width="12.7109375" customWidth="true"/>
     <col min="7" max="7" width="12.7109375" customWidth="true"/>
     <col min="8" max="8" width="12.7109375" customWidth="true"/>
+    <col min="9" max="9" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>3.7070860605234564</v>
+        <v>3.6355338673575743</v>
       </c>
       <c r="C2" s="0">
-        <v>2.6955322272487097</v>
+        <v>0.25678488813161027</v>
       </c>
       <c r="D2" s="0">
-        <v>0.28116566843069535</v>
+        <v>2.6942149542022507</v>
       </c>
       <c r="E2" s="0">
-        <v>0.53025057136291265</v>
+        <v>0.2750174648817475</v>
       </c>
       <c r="F2" s="0">
-        <v>0.46900943414044838</v>
+        <v>0.52442107593206766</v>
       </c>
       <c r="G2" s="0">
-        <v>0.71883433156930465</v>
+        <v>0.47313489480065085</v>
       </c>
       <c r="H2" s="0">
-        <v>0.8478450855197095</v>
+        <v>0.7249825351182525</v>
+      </c>
+      <c r="I2" s="0">
+        <v>0.85146167992064226</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>3.9929950948835313</v>
+        <v>3.796937155822222</v>
       </c>
       <c r="C3" s="0">
-        <v>2.870082762193837</v>
+        <v>0.26818511898755132</v>
       </c>
       <c r="D3" s="0">
-        <v>0.32620792445172492</v>
+        <v>2.8512879068943371</v>
       </c>
       <c r="E3" s="0">
-        <v>0.57114614981782452</v>
+        <v>0.29997889642121928</v>
       </c>
       <c r="F3" s="0">
-        <v>0.49938037417075393</v>
+        <v>0.54770329232278614</v>
       </c>
       <c r="G3" s="0">
-        <v>0.67379207554827514</v>
+        <v>0.50071869795343338</v>
       </c>
       <c r="H3" s="0">
-        <v>0.82354906423438923</v>
+        <v>0.70002110357878067</v>
+      </c>
+      <c r="I3" s="0">
+        <v>0.83720173038329482</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>4.0028793741936211</v>
+        <v>3.7530000486401098</v>
       </c>
       <c r="C4" s="0">
-        <v>2.9386268355159602</v>
+        <v>0.26508175492487912</v>
       </c>
       <c r="D4" s="0">
-        <v>0.3278249166708696</v>
+        <v>2.7829367920920838</v>
       </c>
       <c r="E4" s="0">
-        <v>0.57255996775086326</v>
+        <v>0.29307651929846779</v>
       </c>
       <c r="F4" s="0">
-        <v>0.51130670794540267</v>
+        <v>0.54136542122531961</v>
       </c>
       <c r="G4" s="0">
-        <v>0.67217508332913045</v>
+        <v>0.4887154621087838</v>
       </c>
       <c r="H4" s="0">
-        <v>0.81994867922785919</v>
+        <v>0.70692348070153221</v>
+      </c>
+      <c r="I4" s="0">
+        <v>0.84083194130625505</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated results: salinity experiments 2016-2019 - Added results plot - Added trained model - Added updated dataset
</commit_message>
<xml_diff>
--- a/Parameters-Estimation/Salinity_Estimation/1-Trained-Models/training_test_2016_2019/Results-salinity-calibration-model-k-10.xlsx
+++ b/Parameters-Estimation/Salinity_Estimation/1-Trained-Models/training_test_2016_2019/Results-salinity-calibration-model-k-10.xlsx
@@ -13,7 +13,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>random_forest</t>
+  </si>
+  <si>
+    <t>lsboost</t>
+  </si>
+  <si>
+    <t>neural_network</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>NRMSE</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>RSE</t>
+  </si>
+  <si>
+    <t>RRSE</t>
+  </si>
+  <si>
+    <t>RAE</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Corr Coeff</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>random_forest</t>
+  </si>
+  <si>
+    <t>lsboost</t>
+  </si>
+  <si>
+    <t>neural_network</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>NRMSE</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>RSE</t>
+  </si>
+  <si>
+    <t>RRSE</t>
+  </si>
+  <si>
+    <t>RAE</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Corr Coeff</t>
+  </si>
   <si>
     <t>Row</t>
   </si>
@@ -110,118 +182,118 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B2" s="0">
-        <v>3.6355338673575743</v>
+        <v>3.6123774410934022</v>
       </c>
       <c r="C2" s="0">
-        <v>0.25678488813161027</v>
+        <v>0.25803546167868258</v>
       </c>
       <c r="D2" s="0">
-        <v>2.6942149542022507</v>
+        <v>2.6685154490573511</v>
       </c>
       <c r="E2" s="0">
-        <v>0.2750174648817475</v>
+        <v>0.25889930797023619</v>
       </c>
       <c r="F2" s="0">
-        <v>0.52442107593206766</v>
+        <v>0.50882148929682225</v>
       </c>
       <c r="G2" s="0">
-        <v>0.47313489480065085</v>
+        <v>0.4539140156098056</v>
       </c>
       <c r="H2" s="0">
-        <v>0.7249825351182525</v>
+        <v>0.74110069202976381</v>
       </c>
       <c r="I2" s="0">
-        <v>0.85146167992064226</v>
+        <v>0.86088397525680527</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B3" s="0">
-        <v>3.796937155822222</v>
+        <v>3.6765139028616494</v>
       </c>
       <c r="C3" s="0">
-        <v>0.26818511898755132</v>
+        <v>0.26261678846213121</v>
       </c>
       <c r="D3" s="0">
-        <v>2.8512879068943371</v>
+        <v>2.7507392917803912</v>
       </c>
       <c r="E3" s="0">
-        <v>0.29997889642121928</v>
+        <v>0.26817424821395264</v>
       </c>
       <c r="F3" s="0">
-        <v>0.54770329232278614</v>
+        <v>0.51785543177025062</v>
       </c>
       <c r="G3" s="0">
-        <v>0.50071869795343338</v>
+        <v>0.46790027701311443</v>
       </c>
       <c r="H3" s="0">
-        <v>0.70002110357878067</v>
+        <v>0.73182575178604736</v>
       </c>
       <c r="I3" s="0">
-        <v>0.83720173038329482</v>
+        <v>0.85554979588220958</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B4" s="0">
-        <v>3.7530000486401098</v>
+        <v>3.7571622577195241</v>
       </c>
       <c r="C4" s="0">
-        <v>0.26508175492487912</v>
+        <v>0.2683775750407007</v>
       </c>
       <c r="D4" s="0">
-        <v>2.7829367920920838</v>
+        <v>2.7726271779127898</v>
       </c>
       <c r="E4" s="0">
-        <v>0.29307651929846779</v>
+        <v>0.28006868265378426</v>
       </c>
       <c r="F4" s="0">
-        <v>0.54136542122531961</v>
+        <v>0.52921515724115864</v>
       </c>
       <c r="G4" s="0">
-        <v>0.4887154621087838</v>
+        <v>0.471623402652532</v>
       </c>
       <c r="H4" s="0">
-        <v>0.70692348070153221</v>
+        <v>0.71993131734621574</v>
       </c>
       <c r="I4" s="0">
-        <v>0.84083194130625505</v>
+        <v>0.84868114445409182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>